<commit_message>
Update OPS-2023-10 on 15th October
Update OPS-2023-10 on 15th October
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B69BC90-75D7-4078-BC1E-4E1C7A1613B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6FFAB8-ADA3-4FE8-A7C0-C84848B94543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -141,6 +141,7 @@
   <authors>
     <author>DELL</author>
     <author>tc={0AD6A052-2C07-428D-9436-94F3F1356BBB}</author>
+    <author>tc={A959F053-7A77-46D6-85C0-DFD446771A57}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{B1F31DD9-C91E-48D0-B70E-5B89004C5536}">
@@ -177,6 +178,14 @@
 </t>
       </text>
     </comment>
+    <comment ref="F12" authorId="2" shapeId="0" xr:uid="{A959F053-7A77-46D6-85C0-DFD446771A57}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1) Kinematics</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -186,6 +195,7 @@
   <authors>
     <author>DELL</author>
     <author>tc={49AF81F2-A053-4CA1-87C3-A030A1138880}</author>
+    <author>tc={2BAA0285-3F4A-4F27-A31F-6155E6D26C45}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{C5563D1A-BE92-43EE-B4BF-93F6F984BA58}">
@@ -209,12 +219,20 @@
     1) Matrix and Determinants</t>
       </text>
     </comment>
+    <comment ref="F12" authorId="2" shapeId="0" xr:uid="{2BAA0285-3F4A-4F27-A31F-6155E6D26C45}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1) Complex Number</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
   <si>
     <t>Course</t>
   </si>
@@ -422,6 +440,12 @@
   </si>
   <si>
     <t>12 PM - 02 PM</t>
+  </si>
+  <si>
+    <t>10:30 AM - 12:30 PM</t>
+  </si>
+  <si>
+    <t>12:30 PM - 14:30 PM</t>
   </si>
 </sst>
 </file>
@@ -1600,6 +1624,9 @@
     <text xml:space="preserve">1) Units &amp; Dimension
 </text>
   </threadedComment>
+  <threadedComment ref="F12" dT="2023-10-15T08:41:01.60" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{A959F053-7A77-46D6-85C0-DFD446771A57}">
+    <text>1) Kinematics</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1607,6 +1634,9 @@
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="E12" dT="2023-10-14T08:31:37.05" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{49AF81F2-A053-4CA1-87C3-A030A1138880}">
     <text>1) Matrix and Determinants</text>
+  </threadedComment>
+  <threadedComment ref="F12" dT="2023-10-15T08:41:58.21" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{2BAA0285-3F4A-4F27-A31F-6155E6D26C45}">
+    <text>1) Complex Number</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2784,15 +2814,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="7" width="15.88671875" customWidth="1"/>
+    <col min="4" max="5" width="15.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2833,7 +2865,9 @@
       <c r="E4" s="46">
         <v>45213</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="45">
+        <v>45214</v>
+      </c>
       <c r="G4" s="46"/>
       <c r="H4" s="68"/>
       <c r="I4" s="69"/>
@@ -2849,7 +2883,9 @@
       <c r="E5" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="75"/>
+      <c r="F5" s="75" t="s">
+        <v>68</v>
+      </c>
       <c r="G5" s="76"/>
       <c r="H5" s="71"/>
       <c r="I5" s="72"/>
@@ -2869,7 +2905,9 @@
       <c r="E6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="50"/>
+      <c r="F6" s="50" t="s">
+        <v>41</v>
+      </c>
       <c r="G6" s="60"/>
       <c r="H6" s="65"/>
       <c r="I6" s="66"/>
@@ -2978,15 +3016,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
   <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" customWidth="1"/>
-    <col min="4" max="7" width="12.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -3027,7 +3067,9 @@
       <c r="E4" s="46">
         <v>45213</v>
       </c>
-      <c r="F4" s="45"/>
+      <c r="F4" s="45">
+        <v>45214</v>
+      </c>
       <c r="G4" s="46"/>
       <c r="H4" s="68"/>
       <c r="I4" s="69"/>
@@ -3043,7 +3085,9 @@
       <c r="E5" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="F5" s="47"/>
+      <c r="F5" s="75" t="s">
+        <v>69</v>
+      </c>
       <c r="G5" s="47"/>
       <c r="H5" s="71"/>
       <c r="I5" s="72"/>

</xml_diff>

<commit_message>
updated ops for october 2023
updated ops for october 2023
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF28FBC-2EC2-4C62-9355-CBBAE33C3F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAABC29A-381A-41E9-9302-FF96AFC02A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
@@ -143,6 +143,7 @@
     <author>tc={0AD6A052-2C07-428D-9436-94F3F1356BBB}</author>
     <author>tc={A959F053-7A77-46D6-85C0-DFD446771A57}</author>
     <author>tc={80311F38-7035-4BEB-9468-E983E0329170}</author>
+    <author>tc={6F341809-042B-43CA-A915-78E51369449F}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{B1F31DD9-C91E-48D0-B70E-5B89004C5536}">
@@ -196,6 +197,14 @@
 2) Vector revision</t>
       </text>
     </comment>
+    <comment ref="H12" authorId="4" shapeId="0" xr:uid="{6F341809-042B-43CA-A915-78E51369449F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1) Mechanical Properties of Solid</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -207,6 +216,7 @@
     <author>tc={49AF81F2-A053-4CA1-87C3-A030A1138880}</author>
     <author>tc={2BAA0285-3F4A-4F27-A31F-6155E6D26C45}</author>
     <author>tc={34EAED88-6166-48AD-AE9C-51D01C335AB2}</author>
+    <author>tc={1512A9E1-0F13-46B1-81E8-88DBB9C01E78}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{C5563D1A-BE92-43EE-B4BF-93F6F984BA58}">
@@ -247,12 +257,20 @@
 2) Complex Numbers</t>
       </text>
     </comment>
+    <comment ref="H12" authorId="4" shapeId="0" xr:uid="{1512A9E1-0F13-46B1-81E8-88DBB9C01E78}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1) Sequence and series</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
   <si>
     <t>Course</t>
   </si>
@@ -634,7 +652,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1109,11 +1127,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1313,6 +1377,21 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1663,6 +1742,9 @@
     <text>1) Kinemetics
 2) Vector revision</text>
   </threadedComment>
+  <threadedComment ref="H12" dT="2023-10-29T08:43:16.35" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{6F341809-042B-43CA-A915-78E51369449F}">
+    <text>1) Mechanical Properties of Solid</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1677,6 +1759,9 @@
   <threadedComment ref="G12" dT="2023-10-28T08:39:40.71" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{34EAED88-6166-48AD-AE9C-51D01C335AB2}">
     <text>1) AP and GP
 2) Complex Numbers</text>
+  </threadedComment>
+  <threadedComment ref="H12" dT="2023-10-29T08:41:58.56" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{1512A9E1-0F13-46B1-81E8-88DBB9C01E78}">
+    <text>1) Sequence and series</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2856,10 +2941,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DABE7A-7845-46EA-BB0E-44CB73A3B0F1}">
-  <dimension ref="B1:K24"/>
+  <dimension ref="B1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2867,12 +2952,12 @@
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="6" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="77" t="s">
         <v>71</v>
       </c>
@@ -2880,23 +2965,25 @@
       <c r="D2" s="78"/>
       <c r="E2" s="78"/>
       <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
-    </row>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="80"/>
       <c r="C3" s="81"/>
       <c r="D3" s="81"/>
       <c r="E3" s="81"/>
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="81"/>
+      <c r="I3" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="89"/>
       <c r="J3" s="89"/>
-      <c r="K3" s="90"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K3" s="89"/>
+      <c r="L3" s="90"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="84" t="s">
         <v>44</v>
       </c>
@@ -2915,12 +3002,15 @@
       <c r="G4" s="46">
         <v>45227</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
+      <c r="H4" s="46">
+        <v>45228</v>
+      </c>
+      <c r="I4" s="68"/>
       <c r="J4" s="69"/>
-      <c r="K4" s="70"/>
-    </row>
-    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="69"/>
+      <c r="L4" s="70"/>
+    </row>
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="85"/>
       <c r="C5" s="87"/>
       <c r="D5" s="74" t="s">
@@ -2935,12 +3025,15 @@
       <c r="G5" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="72"/>
+      <c r="H5" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="71"/>
       <c r="J5" s="72"/>
-      <c r="K5" s="73"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K5" s="72"/>
+      <c r="L5" s="73"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="38">
         <v>1</v>
       </c>
@@ -2959,12 +3052,15 @@
       <c r="G6" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="66"/>
+      <c r="H6" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="65"/>
       <c r="J6" s="66"/>
-      <c r="K6" s="67"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="66"/>
+      <c r="L6" s="67"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="40">
         <v>2</v>
       </c>
@@ -2973,12 +3069,13 @@
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="52"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="63"/>
       <c r="J7" s="52"/>
-      <c r="K7" s="53"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="40">
         <v>3</v>
       </c>
@@ -2987,12 +3084,13 @@
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
       <c r="G8" s="61"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="52"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="63"/>
       <c r="J8" s="52"/>
-      <c r="K8" s="53"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="52"/>
+      <c r="L8" s="53"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="40">
         <v>4</v>
       </c>
@@ -3001,12 +3099,13 @@
       <c r="E9" s="52"/>
       <c r="F9" s="52"/>
       <c r="G9" s="61"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="52"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="63"/>
       <c r="J9" s="52"/>
-      <c r="K9" s="53"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K9" s="52"/>
+      <c r="L9" s="53"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="40">
         <v>5</v>
       </c>
@@ -3015,12 +3114,13 @@
       <c r="E10" s="52"/>
       <c r="F10" s="52"/>
       <c r="G10" s="61"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="52"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="63"/>
       <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
-    </row>
-    <row r="11" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K10" s="52"/>
+      <c r="L10" s="53"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="42">
         <v>6</v>
       </c>
@@ -3029,12 +3129,13 @@
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="62"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="55"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="64"/>
       <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
-    </row>
-    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K11" s="55"/>
+      <c r="L11" s="56"/>
+    </row>
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="82" t="s">
         <v>43</v>
       </c>
@@ -3042,17 +3143,18 @@
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
-    </row>
-    <row r="24" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J24" t="s">
+      <c r="G12" s="91"/>
+      <c r="H12" s="97"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K24" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="I3:L3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>
@@ -3064,10 +3166,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3075,12 +3177,12 @@
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" customWidth="1"/>
     <col min="4" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="77" t="s">
         <v>62</v>
       </c>
@@ -3088,23 +3190,25 @@
       <c r="D2" s="78"/>
       <c r="E2" s="78"/>
       <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
-    </row>
-    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="80"/>
       <c r="C3" s="81"/>
       <c r="D3" s="81"/>
       <c r="E3" s="81"/>
       <c r="F3" s="81"/>
       <c r="G3" s="81"/>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="81"/>
+      <c r="I3" s="88" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="89"/>
       <c r="J3" s="89"/>
-      <c r="K3" s="90"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K3" s="89"/>
+      <c r="L3" s="90"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="84" t="s">
         <v>44</v>
       </c>
@@ -3123,12 +3227,15 @@
       <c r="G4" s="46">
         <v>45227</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
+      <c r="H4" s="46">
+        <v>45228</v>
+      </c>
+      <c r="I4" s="68"/>
       <c r="J4" s="69"/>
-      <c r="K4" s="70"/>
-    </row>
-    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="69"/>
+      <c r="L4" s="70"/>
+    </row>
+    <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="85"/>
       <c r="C5" s="87"/>
       <c r="D5" s="74" t="s">
@@ -3143,12 +3250,15 @@
       <c r="G5" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="72"/>
+      <c r="H5" s="93" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="71"/>
       <c r="J5" s="72"/>
-      <c r="K5" s="73"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K5" s="72"/>
+      <c r="L5" s="73"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="38">
         <v>1</v>
       </c>
@@ -3167,12 +3277,15 @@
       <c r="G6" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="66"/>
+      <c r="H6" s="94" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="92"/>
       <c r="J6" s="66"/>
-      <c r="K6" s="67"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="66"/>
+      <c r="L6" s="67"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="40">
         <v>2</v>
       </c>
@@ -3181,12 +3294,13 @@
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="52"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="51"/>
       <c r="J7" s="52"/>
-      <c r="K7" s="53"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="40">
         <v>3</v>
       </c>
@@ -3195,12 +3309,13 @@
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
       <c r="G8" s="61"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="52"/>
+      <c r="H8" s="95"/>
+      <c r="I8" s="51"/>
       <c r="J8" s="52"/>
-      <c r="K8" s="53"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K8" s="52"/>
+      <c r="L8" s="53"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="40">
         <v>4</v>
       </c>
@@ -3209,12 +3324,13 @@
       <c r="E9" s="52"/>
       <c r="F9" s="52"/>
       <c r="G9" s="61"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="52"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="52"/>
-      <c r="K9" s="53"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K9" s="52"/>
+      <c r="L9" s="53"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="40">
         <v>5</v>
       </c>
@@ -3223,12 +3339,13 @@
       <c r="E10" s="52"/>
       <c r="F10" s="52"/>
       <c r="G10" s="61"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="52"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="52"/>
-      <c r="K10" s="53"/>
-    </row>
-    <row r="11" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K10" s="52"/>
+      <c r="L10" s="53"/>
+    </row>
+    <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="42">
         <v>6</v>
       </c>
@@ -3237,12 +3354,13 @@
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="62"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="55"/>
+      <c r="H11" s="95"/>
+      <c r="I11" s="54"/>
       <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
-    </row>
-    <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K11" s="55"/>
+      <c r="L11" s="56"/>
+    </row>
+    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="82" t="s">
         <v>43</v>
       </c>
@@ -3250,12 +3368,13 @@
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
-      <c r="G12" s="37"/>
+      <c r="G12" s="91"/>
+      <c r="H12" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B2:H3"/>
+    <mergeCell ref="I3:L3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B12:C12"/>

</xml_diff>

<commit_message>
Ops updated for october and news Ops for november 2023 created
Ops updated for october and news Ops for november 2023 created
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAABC29A-381A-41E9-9302-FF96AFC02A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8D647A-F7F9-4921-864D-75B12CAE08B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -46,6 +46,7 @@
   <authors>
     <author>DELL</author>
     <author>tc={FB362581-5BC1-4323-BA14-6A72194D1DAC}</author>
+    <author>tc={919C3780-69CB-4E01-A0F9-3C3DA9401F69}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{E303604D-949B-4EC3-A89E-AB3D1B0AFF2D}">
@@ -80,6 +81,14 @@
     V.S.E.P.R Theory, Bond Angle , Bond Polarity, Dipole Moment</t>
       </text>
     </comment>
+    <comment ref="G12" authorId="2" shapeId="0" xr:uid="{919C3780-69CB-4E01-A0F9-3C3DA9401F69}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Teacher was on Durga Puja leave</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -89,6 +98,7 @@
   <authors>
     <author>DELL</author>
     <author>tc={5E4F6515-A34B-476F-B8AA-CC1C8A79FDE2}</author>
+    <author>tc={E520D902-3900-47AB-9DF2-61CF9FCE8922}</author>
   </authors>
   <commentList>
     <comment ref="D12" authorId="0" shapeId="0" xr:uid="{33CEDD93-340D-4DFF-8853-769F5B2FE230}">
@@ -130,6 +140,14 @@
 2) Bond Angle 
 3) Bond Polarity
 4) Dipole Moment</t>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="2" shapeId="0" xr:uid="{E520D902-3900-47AB-9DF2-61CF9FCE8922}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Teacher was on Durga Puja leave</t>
       </text>
     </comment>
   </commentList>
@@ -270,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
   <si>
     <t>Course</t>
   </si>
@@ -409,9 +427,6 @@
   <si>
     <t>Faculty: Subrata Ghosh     ||     Batct: B1: NEET &amp; IIT Crash Course Chemistry
 Timing: Thursday 4-6pm     ||     Start date: 07/Sep/2023</t>
-  </si>
-  <si>
-    <t>2-4pm</t>
   </si>
   <si>
     <t>Practice Tests Marks</t>
@@ -1177,7 +1192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1335,6 +1350,18 @@
     <xf numFmtId="14" fontId="8" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1377,21 +1404,6 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="6" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1715,6 +1727,9 @@
   <threadedComment ref="E12" dT="2023-10-12T12:03:06.44" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{FB362581-5BC1-4323-BA14-6A72194D1DAC}">
     <text>V.S.E.P.R Theory, Bond Angle , Bond Polarity, Dipole Moment</text>
   </threadedComment>
+  <threadedComment ref="G12" dT="2023-10-30T06:19:15.10" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{919C3780-69CB-4E01-A0F9-3C3DA9401F69}">
+    <text>Teacher was on Durga Puja leave</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1725,6 +1740,9 @@
 2) Bond Angle 
 3) Bond Polarity
 4) Dipole Moment</text>
+  </threadedComment>
+  <threadedComment ref="G12" dT="2023-10-30T06:19:33.24" personId="{7AB4B534-9F76-496B-ABA0-40BBDE98DE46}" id="{E520D902-3900-47AB-9DF2-61CF9FCE8922}">
+    <text>Teacher was on Durga Puja leave</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1785,7 +1803,7 @@
   <dimension ref="B1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1793,7 +1811,7 @@
     <col min="1" max="1" width="4.109375" customWidth="1"/>
     <col min="2" max="2" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -1989,7 +2007,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" s="8">
         <v>1</v>
@@ -2476,7 +2494,7 @@
   <cols>
     <col min="2" max="2" width="3.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -2484,28 +2502,28 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
       <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
       <c r="I1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
@@ -2513,19 +2531,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="57">
         <v>45202</v>
       </c>
       <c r="F2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" t="s">
         <v>60</v>
-      </c>
-      <c r="G2" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2538,7 +2556,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2553,34 +2571,34 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="88" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="90"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="94" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="96"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -2595,16 +2613,14 @@
       <c r="G4" s="58">
         <v>45225</v>
       </c>
-      <c r="H4" s="68">
-        <v>45226</v>
-      </c>
+      <c r="H4" s="68"/>
       <c r="I4" s="69"/>
       <c r="J4" s="69"/>
       <c r="K4" s="70"/>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="85"/>
-      <c r="C5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="47" t="s">
         <v>39</v>
       </c>
@@ -2612,14 +2628,12 @@
         <v>39</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="71" t="s">
-        <v>46</v>
-      </c>
+      <c r="H5" s="71"/>
       <c r="I5" s="72"/>
       <c r="J5" s="72"/>
       <c r="K5" s="73"/>
@@ -2640,7 +2654,9 @@
       <c r="F6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="60"/>
+      <c r="G6" s="60" t="s">
+        <v>42</v>
+      </c>
       <c r="H6" s="65"/>
       <c r="I6" s="66"/>
       <c r="J6" s="66"/>
@@ -2717,10 +2733,10 @@
       <c r="K11" s="56"/>
     </row>
     <row r="12" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -2743,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A980A2-087E-4BDA-864D-B7CC763A9F65}">
   <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2757,34 +2773,34 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="77" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="79"/>
+      <c r="B2" s="83" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="85"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="88" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="90"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="94" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="96"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -2805,19 +2821,19 @@
       <c r="K4" s="70"/>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="85"/>
-      <c r="C5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="71"/>
       <c r="I5" s="72"/>
@@ -2840,7 +2856,9 @@
       <c r="F6" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="60"/>
+      <c r="G6" s="60" t="s">
+        <v>42</v>
+      </c>
       <c r="H6" s="65"/>
       <c r="I6" s="66"/>
       <c r="J6" s="66"/>
@@ -2917,10 +2935,10 @@
       <c r="K11" s="56"/>
     </row>
     <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -2958,36 +2976,36 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="77" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
+      <c r="B2" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="88" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="90"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="94" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="96"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -3011,22 +3029,22 @@
       <c r="L4" s="70"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="85"/>
-      <c r="C5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="74" t="s">
         <v>39</v>
       </c>
       <c r="E5" s="75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5" s="76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H5" s="76" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="71"/>
       <c r="J5" s="72"/>
@@ -3129,26 +3147,26 @@
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="62"/>
-      <c r="H11" s="96"/>
+      <c r="H11" s="81"/>
       <c r="I11" s="64"/>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
       <c r="L11" s="56"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="97"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="82"/>
     </row>
     <row r="24" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3168,7 +3186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0268C353-496F-4BD6-A7EF-D042619A03C3}">
   <dimension ref="B1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -3183,36 +3201,36 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="77" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="79"/>
+      <c r="B2" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="88" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="90"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="94" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="96"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="92" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -3236,22 +3254,22 @@
       <c r="L4" s="70"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="85"/>
-      <c r="C5" s="87"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="74" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="93" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="H5" s="79" t="s">
+        <v>72</v>
       </c>
       <c r="I5" s="71"/>
       <c r="J5" s="72"/>
@@ -3277,10 +3295,10 @@
       <c r="G6" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="94" t="s">
+      <c r="H6" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="I6" s="92"/>
+      <c r="I6" s="78"/>
       <c r="J6" s="66"/>
       <c r="K6" s="66"/>
       <c r="L6" s="67"/>
@@ -3294,7 +3312,7 @@
       <c r="E7" s="52"/>
       <c r="F7" s="52"/>
       <c r="G7" s="61"/>
-      <c r="H7" s="95"/>
+      <c r="H7" s="80"/>
       <c r="I7" s="51"/>
       <c r="J7" s="52"/>
       <c r="K7" s="52"/>
@@ -3309,7 +3327,7 @@
       <c r="E8" s="52"/>
       <c r="F8" s="52"/>
       <c r="G8" s="61"/>
-      <c r="H8" s="95"/>
+      <c r="H8" s="80"/>
       <c r="I8" s="51"/>
       <c r="J8" s="52"/>
       <c r="K8" s="52"/>
@@ -3324,7 +3342,7 @@
       <c r="E9" s="52"/>
       <c r="F9" s="52"/>
       <c r="G9" s="61"/>
-      <c r="H9" s="95"/>
+      <c r="H9" s="80"/>
       <c r="I9" s="51"/>
       <c r="J9" s="52"/>
       <c r="K9" s="52"/>
@@ -3339,7 +3357,7 @@
       <c r="E10" s="52"/>
       <c r="F10" s="52"/>
       <c r="G10" s="61"/>
-      <c r="H10" s="95"/>
+      <c r="H10" s="80"/>
       <c r="I10" s="51"/>
       <c r="J10" s="52"/>
       <c r="K10" s="52"/>
@@ -3354,22 +3372,22 @@
       <c r="E11" s="55"/>
       <c r="F11" s="55"/>
       <c r="G11" s="62"/>
-      <c r="H11" s="95"/>
+      <c r="H11" s="80"/>
       <c r="I11" s="54"/>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
       <c r="L11" s="56"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="88" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="95"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Some docs checked in
Some docs checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8D647A-F7F9-4921-864D-75B12CAE08B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E27579-2095-418F-B805-28BBB344250A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="8" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="B2" sheetId="4" r:id="rId7"/>
     <sheet name="B3" sheetId="5" r:id="rId8"/>
     <sheet name="B4" sheetId="9" r:id="rId9"/>
+    <sheet name="Chemistry-Syllabus" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -288,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="103">
   <si>
     <t>Course</t>
   </si>
@@ -511,6 +512,96 @@
   </si>
   <si>
     <t>12:30 PM -14:30 PM</t>
+  </si>
+  <si>
+    <t>SlNo</t>
+  </si>
+  <si>
+    <t>Topics</t>
+  </si>
+  <si>
+    <t>Some Basic Concepts of Chemistry</t>
+  </si>
+  <si>
+    <t>Solid State</t>
+  </si>
+  <si>
+    <t>Solutions</t>
+  </si>
+  <si>
+    <t>Sahesta</t>
+  </si>
+  <si>
+    <t>Prottoy</t>
+  </si>
+  <si>
+    <t>Electrochemistry</t>
+  </si>
+  <si>
+    <t>Chemical Kinetics</t>
+  </si>
+  <si>
+    <t>Surface Chemistry</t>
+  </si>
+  <si>
+    <t>Structure of Atom</t>
+  </si>
+  <si>
+    <t>Classification of elements and periodicity of properties</t>
+  </si>
+  <si>
+    <t>Chemical Bonding and Molecular State</t>
+  </si>
+  <si>
+    <t>States of Matter Gases and Liquids</t>
+  </si>
+  <si>
+    <t>Thermodynamics</t>
+  </si>
+  <si>
+    <t>Equilibrium</t>
+  </si>
+  <si>
+    <t>Redox Reactions</t>
+  </si>
+  <si>
+    <t>Hydrogen</t>
+  </si>
+  <si>
+    <t>S-Block of elements (Alkali and Alkaline Earth Materials)</t>
+  </si>
+  <si>
+    <t>Some P-Block Elements</t>
+  </si>
+  <si>
+    <t>Environmental Chemistry</t>
+  </si>
+  <si>
+    <t>P-Block Elements</t>
+  </si>
+  <si>
+    <t>D and F Block Elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coordination Compounds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haloalkanes and Haloarenes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcohols, Phenols and Ethers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic compounds containing Nitrogen  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomolecules </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polymers  </t>
+  </si>
+  <si>
+    <t>Chemistry in Everyday Life</t>
   </si>
 </sst>
 </file>
@@ -520,7 +611,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -604,12 +695,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1192,7 +1277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1403,6 +1488,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1798,6 +1886,247 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367A9178-56D8-4567-9604-94ED4820331C}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.77734375" style="97" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="97" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="97">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="97">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="97">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="97">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="97">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="97">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="97">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="97">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="97">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="97">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="97">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="97">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="97">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="97">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="97">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="97">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="97">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="97">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="97">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="97">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="97">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="97">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="97">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="97">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="97">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="97">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66DF67B1-7A31-46BB-8007-D9F915FBEBAF}">
   <dimension ref="B1:M15"/>
@@ -2759,16 +3088,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23A980A2-087E-4BDA-864D-B7CC763A9F65}">
   <dimension ref="B1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="5" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Ops and mock test planning docs checked in
Ops and mock test planning docs checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
+++ b/Offline/BusinessManagement/Ops/Ops-2023-10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Ops\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E27579-2095-418F-B805-28BBB344250A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B07604-9791-49A2-979C-A981804FD752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="9" xr2:uid="{C08D87AB-705E-4371-9352-7E8E74F7A2B7}"/>
   </bookViews>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="104">
   <si>
     <t>Course</t>
   </si>
@@ -529,12 +529,6 @@
     <t>Solutions</t>
   </si>
   <si>
-    <t>Sahesta</t>
-  </si>
-  <si>
-    <t>Prottoy</t>
-  </si>
-  <si>
     <t>Electrochemistry</t>
   </si>
   <si>
@@ -602,6 +596,15 @@
   </si>
   <si>
     <t>Chemistry in Everyday Life</t>
+  </si>
+  <si>
+    <t>Coverage Percentage</t>
+  </si>
+  <si>
+    <t>Prottoy (Covered(0-1)</t>
+  </si>
+  <si>
+    <t>Sahesta  (Covered(0-1))</t>
   </si>
 </sst>
 </file>
@@ -611,7 +614,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,6 +698,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1277,7 +1289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1447,6 +1459,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1488,9 +1511,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1888,238 +1908,409 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{367A9178-56D8-4567-9604-94ED4820331C}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="97" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" style="83" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="83" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="86" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="87" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" t="s">
-        <v>79</v>
+      <c r="C1" s="87" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="86" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="97">
+      <c r="A3" s="83">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>75</v>
       </c>
+      <c r="C3" s="83">
+        <v>0</v>
+      </c>
+      <c r="D3" s="83">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="97">
+      <c r="A4" s="83">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>76</v>
       </c>
+      <c r="C4" s="83">
+        <v>0</v>
+      </c>
+      <c r="D4" s="83">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="97">
+      <c r="A5" s="83">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
       </c>
+      <c r="C5" s="83">
+        <v>0</v>
+      </c>
+      <c r="D5" s="83">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="97">
+      <c r="A6" s="83">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="83">
+        <v>0</v>
+      </c>
+      <c r="D6" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="83">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="83">
+        <v>0</v>
+      </c>
+      <c r="D7" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="83">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="97">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" s="83">
+        <v>0</v>
+      </c>
+      <c r="D8" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="83">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="97">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" s="83">
+        <v>0</v>
+      </c>
+      <c r="D9" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="83">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="97">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10" s="83">
+        <v>0</v>
+      </c>
+      <c r="D10" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="83">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="97">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11" s="83">
+        <v>0</v>
+      </c>
+      <c r="D11" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="83">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="97">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C12" s="83">
+        <v>0</v>
+      </c>
+      <c r="D12" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="83">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="97">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C13" s="83">
+        <v>0</v>
+      </c>
+      <c r="D13" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="83">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="97">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C14" s="83">
+        <v>0</v>
+      </c>
+      <c r="D14" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="83">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="97">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C15" s="83">
+        <v>0</v>
+      </c>
+      <c r="D15" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="83">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="97">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C16" s="83">
+        <v>0</v>
+      </c>
+      <c r="D16" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="83">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="97">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C17" s="83">
+        <v>0</v>
+      </c>
+      <c r="D17" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="83">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="97">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C18" s="83">
+        <v>0</v>
+      </c>
+      <c r="D18" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="83">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="97">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C19" s="83">
+        <v>0</v>
+      </c>
+      <c r="D19" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="83">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="97">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C20" s="83">
+        <v>0</v>
+      </c>
+      <c r="D20" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="83">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="97">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C21" s="83">
+        <v>0</v>
+      </c>
+      <c r="D21" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="83">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="97">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C22" s="83">
+        <v>0</v>
+      </c>
+      <c r="D22" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="83">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="97">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C23" s="83">
+        <v>0</v>
+      </c>
+      <c r="D23" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="83">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="97">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C24" s="83">
+        <v>0</v>
+      </c>
+      <c r="D24" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="83">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="97">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C25" s="83">
+        <v>0</v>
+      </c>
+      <c r="D25" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="83">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="97">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C26" s="83">
+        <v>0</v>
+      </c>
+      <c r="D26" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="83">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="97">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C27" s="83">
+        <v>0</v>
+      </c>
+      <c r="D27" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="83">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="97">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C28" s="83">
+        <v>0</v>
+      </c>
+      <c r="D28" s="83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="84" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="97">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>102</v>
+      <c r="C30" s="85">
+        <f>ROUND((SUM(C3:C28)/26) * 100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="85">
+        <f>ROUND((SUM(D3:D28)/26) * 100,2)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2900,34 +3091,34 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="85"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="90"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="94" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="96"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="101"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="97" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -2948,8 +3139,8 @@
       <c r="K4" s="70"/>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="91"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="47" t="s">
         <v>39</v>
       </c>
@@ -3062,10 +3253,10 @@
       <c r="K11" s="56"/>
     </row>
     <row r="12" spans="2:11" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="89"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -3089,7 +3280,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3102,34 +3293,34 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="85"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="90"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="94" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="96"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="101"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="97" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -3150,8 +3341,8 @@
       <c r="K4" s="70"/>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="91"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="47" t="s">
         <v>47</v>
       </c>
@@ -3264,10 +3455,10 @@
       <c r="K11" s="56"/>
     </row>
     <row r="12" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="89"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -3305,36 +3496,36 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="90"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="94" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="96"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="101"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="97" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -3358,8 +3549,8 @@
       <c r="L4" s="70"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="91"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="74" t="s">
         <v>39</v>
       </c>
@@ -3483,10 +3674,10 @@
       <c r="L11" s="56"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="89"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
@@ -3530,36 +3721,36 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="85"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="90"/>
     </row>
     <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="94" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="96"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="101"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="97" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="45">
@@ -3583,8 +3774,8 @@
       <c r="L4" s="70"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="91"/>
-      <c r="C5" s="93"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="98"/>
       <c r="D5" s="74" t="s">
         <v>62</v>
       </c>
@@ -3708,10 +3899,10 @@
       <c r="L11" s="56"/>
     </row>
     <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="88" t="s">
+      <c r="B12" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="89"/>
+      <c r="C12" s="94"/>
       <c r="D12" s="44"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>

</xml_diff>